<commit_message>
performance and scaling plots for MPI-only jobs are included
</commit_message>
<xml_diff>
--- a/data/scale-lj/scaling-data.xlsx
+++ b/data/scale-lj/scaling-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prithwish/Documents/Work/HPC_Carpentries/git/tuning_lammps/data/scale-lj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B65D99-80FA-6046-9FF6-ACAE03A7D415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B1879-42F3-DF4B-BC79-568896BD359C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40080" yWindow="4040" windowWidth="28040" windowHeight="17440" xr2:uid="{507AB68B-F224-A949-A11C-23FEE6C57D7F}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AF206D-1213-A14C-B085-D3411139F9F8}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,6 +852,93 @@
         <v>0.84</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>288</v>
+      </c>
+      <c r="B16">
+        <v>3568.78</v>
+      </c>
+      <c r="C16">
+        <v>2.8020799999999998E-2</v>
+      </c>
+      <c r="D16">
+        <v>39.14</v>
+      </c>
+      <c r="E16">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F16">
+        <v>32.07</v>
+      </c>
+      <c r="G16">
+        <v>22.52</v>
+      </c>
+      <c r="H16">
+        <v>1.02</v>
+      </c>
+      <c r="I16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>336</v>
+      </c>
+      <c r="B17">
+        <v>3781.1210000000001</v>
+      </c>
+      <c r="C17">
+        <v>2.6447200000000001E-2</v>
+      </c>
+      <c r="D17">
+        <v>35.51</v>
+      </c>
+      <c r="E17">
+        <v>4.05</v>
+      </c>
+      <c r="F17">
+        <v>36.11</v>
+      </c>
+      <c r="G17">
+        <v>21.82</v>
+      </c>
+      <c r="H17">
+        <v>1.54</v>
+      </c>
+      <c r="I17">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>384</v>
+      </c>
+      <c r="B18">
+        <v>4025.6379999999999</v>
+      </c>
+      <c r="C18">
+        <v>2.48408E-2</v>
+      </c>
+      <c r="D18">
+        <v>32.85</v>
+      </c>
+      <c r="E18">
+        <v>3.89</v>
+      </c>
+      <c r="F18">
+        <v>37.869999999999997</v>
+      </c>
+      <c r="G18">
+        <v>23.52</v>
+      </c>
+      <c r="H18">
+        <v>0.95</v>
+      </c>
+      <c r="I18">
+        <v>0.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>